<commit_message>
modification for login - eInvoice execution
</commit_message>
<xml_diff>
--- a/Datasheet/eInvoice_data.xlsx
+++ b/Datasheet/eInvoice_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17430" windowHeight="8385" tabRatio="675" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20430" windowHeight="8385" tabRatio="675" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="ProcessForm" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G15"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="173">
   <si>
     <t>invoice_name</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t>iContract</t>
+  </si>
+  <si>
+    <t>ZCS Production</t>
   </si>
 </sst>
 </file>
@@ -1629,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1849,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
@@ -1862,6 +1865,26 @@
       </c>
       <c r="F11" s="1" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1889,9 +1912,11 @@
     <hyperlink ref="F10" r:id="rId21"/>
     <hyperlink ref="D11" r:id="rId22"/>
     <hyperlink ref="F11" r:id="rId23"/>
+    <hyperlink ref="D12" r:id="rId24"/>
+    <hyperlink ref="F12" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed Rainbow navigation with few other functions
</commit_message>
<xml_diff>
--- a/Datasheet/eInvoice_data.xlsx
+++ b/Datasheet/eInvoice_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20430" windowHeight="8385" tabRatio="675" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="675" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="PurchaseOrders" sheetId="23" r:id="rId7"/>
     <sheet name="ViewInvoice" sheetId="6" r:id="rId8"/>
     <sheet name="Workflow" sheetId="12" r:id="rId9"/>
-    <sheet name="Reconcile New Statement" sheetId="13" r:id="rId10"/>
+    <sheet name="Reconciliation" sheetId="13" r:id="rId10"/>
     <sheet name="MyReports" sheetId="14" r:id="rId11"/>
     <sheet name="Reports" sheetId="15" r:id="rId12"/>
     <sheet name="Uploads" sheetId="17" r:id="rId13"/>
@@ -25,12 +25,12 @@
     <sheet name="ProcessForm" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I32"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="173">
   <si>
     <t>invoice_name</t>
   </si>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2046,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,10 +2056,9 @@
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2082,24 +2081,21 @@
         <v>130</v>
       </c>
       <c r="G1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2122,25 +2118,22 @@
       <c r="F2" t="s">
         <v>139</v>
       </c>
-      <c r="G2">
-        <v>70</v>
+      <c r="G2" t="s">
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
         <v>29</v>
       </c>
+      <c r="I2">
+        <v>32189</v>
+      </c>
       <c r="J2">
-        <v>32189</v>
-      </c>
-      <c r="K2">
         <v>1000</v>
       </c>
+      <c r="K2" t="s">
+        <v>140</v>
+      </c>
       <c r="L2" t="s">
-        <v>140</v>
-      </c>
-      <c r="M2" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added @BeforeMethod, Added String...navigationTabs to felicitate navigation
</commit_message>
<xml_diff>
--- a/Datasheet/eInvoice_data.xlsx
+++ b/Datasheet/eInvoice_data.xlsx
@@ -4,33 +4,37 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="675" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="675" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
     <sheet name="Configuration" sheetId="24" r:id="rId2"/>
     <sheet name="Login" sheetId="2" r:id="rId3"/>
     <sheet name="Invoices" sheetId="11" r:id="rId4"/>
-    <sheet name="InvoiceNonPO" sheetId="21" r:id="rId5"/>
-    <sheet name="CreditMemowithoutReference" sheetId="22" r:id="rId6"/>
-    <sheet name="PurchaseOrders" sheetId="23" r:id="rId7"/>
-    <sheet name="ViewInvoice" sheetId="6" r:id="rId8"/>
-    <sheet name="Workflow" sheetId="12" r:id="rId9"/>
-    <sheet name="Reconciliation" sheetId="13" r:id="rId10"/>
-    <sheet name="MyReports" sheetId="14" r:id="rId11"/>
-    <sheet name="Reports" sheetId="15" r:id="rId12"/>
-    <sheet name="Uploads" sheetId="17" r:id="rId13"/>
-    <sheet name="Batches" sheetId="18" r:id="rId14"/>
-    <sheet name="NewBatch" sheetId="19" r:id="rId15"/>
-    <sheet name="ProcessForm" sheetId="20" r:id="rId16"/>
+    <sheet name="Approvals" sheetId="25" r:id="rId5"/>
+    <sheet name="MySettings" sheetId="26" r:id="rId6"/>
+    <sheet name="InvoiceNonPO" sheetId="21" r:id="rId7"/>
+    <sheet name="CreditMemowithoutReference" sheetId="22" r:id="rId8"/>
+    <sheet name="CreditMemoAgainstPO" sheetId="27" r:id="rId9"/>
+    <sheet name="InvoiceAgainstPO" sheetId="28" r:id="rId10"/>
+    <sheet name="PurchaseOrders" sheetId="23" r:id="rId11"/>
+    <sheet name="ViewInvoice" sheetId="6" r:id="rId12"/>
+    <sheet name="Workflow" sheetId="12" r:id="rId13"/>
+    <sheet name="Reconciliation" sheetId="13" r:id="rId14"/>
+    <sheet name="MyReports" sheetId="14" r:id="rId15"/>
+    <sheet name="Reports" sheetId="15" r:id="rId16"/>
+    <sheet name="Uploads" sheetId="17" r:id="rId17"/>
+    <sheet name="Batches" sheetId="18" r:id="rId18"/>
+    <sheet name="NewBatch" sheetId="19" r:id="rId19"/>
+    <sheet name="ProcessForm" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I32"/>
+  <oleSize ref="A1:G32"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="181">
   <si>
     <t>invoice_name</t>
   </si>
@@ -549,6 +553,30 @@
   </si>
   <si>
     <t>ZCS Production</t>
+  </si>
+  <si>
+    <t>SubTab</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Invoices</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t>All Requests</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>My Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag </t>
   </si>
 </sst>
 </file>
@@ -923,7 +951,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,59 +1115,34 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="2">
-        <v>43458</v>
-      </c>
-      <c r="F2" t="s">
-        <v>79</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1149,17 +1152,88 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,13 +1241,13 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,13 +1255,151 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43458</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1195,47 +1407,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1243,12 +1454,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1519,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1277,58 +1535,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>846704</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>84</v>
-      </c>
-      <c r="D2">
-        <v>846704</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1336,233 +1590,71 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
         <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" t="s">
-        <v>106</v>
-      </c>
-      <c r="M1" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" t="s">
-        <v>108</v>
-      </c>
-      <c r="O1" t="s">
-        <v>109</v>
-      </c>
-      <c r="P1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>111</v>
-      </c>
-      <c r="R1" t="s">
-        <v>112</v>
-      </c>
-      <c r="S1" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" t="s">
-        <v>123</v>
-      </c>
-      <c r="M2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N2" t="s">
-        <v>125</v>
-      </c>
-      <c r="O2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P2">
-        <v>6</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1623,6 +1715,164 @@
       </c>
       <c r="D3" t="s">
         <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" t="s">
+        <v>114</v>
+      </c>
+      <c r="S1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>96</v>
+      </c>
+      <c r="T2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1922,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="P1" sqref="P1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,7 +2195,7 @@
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1991,8 +2241,14 @@
       <c r="O1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2034,6 +2290,12 @@
       </c>
       <c r="O2">
         <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2044,9 +2306,86 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -2142,12 +2481,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="M1" sqref="M1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2500,7 @@
     <col min="12" max="12" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -2198,8 +2537,14 @@
       <c r="L1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2236,130 +2581,11 @@
       <c r="L2" t="s">
         <v>141</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="M2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="N2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2370,63 +2596,37 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
iManage files added to the project
</commit_message>
<xml_diff>
--- a/Datasheet/eInvoice_data.xlsx
+++ b/Datasheet/eInvoice_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="675" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="675" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,11 @@
     <sheet name="ProcessForm" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F32"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="183">
   <si>
     <t>invoice_name</t>
   </si>
@@ -577,6 +576,12 @@
   </si>
   <si>
     <t xml:space="preserve">flag </t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>GLAccount</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1291,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -1300,7 +1305,7 @@
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1320,7 +1325,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1348,7 +1353,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -1362,7 +1367,7 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1387,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1409,7 +1414,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -1421,7 +1426,7 @@
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1435,7 +1440,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1456,7 +1461,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1468,7 +1473,7 @@
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1537,7 +1542,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
@@ -1545,7 +1550,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1565,7 +1570,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1592,7 +1597,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -1605,7 +1610,7 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1724,7 +1729,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -1751,7 +1756,7 @@
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1813,7 +1818,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1884,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2174,7 +2179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1:Q2"/>
     </sheetView>
   </sheetViews>
@@ -2349,7 +2354,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,7 +2405,7 @@
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -2435,10 +2440,16 @@
         <v>136</v>
       </c>
       <c r="L1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="M1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2455,7 +2466,7 @@
         <v>43270</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="G2" t="s">
         <v>23</v>
@@ -2474,6 +2485,12 @@
       </c>
       <c r="L2" t="s">
         <v>141</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>